<commit_message>
Update global battery, wind/solar capacity to EU start year
</commit_message>
<xml_diff>
--- a/InputData/endo-learn/BGBSC/BAU Global Battery Storage Cap.xlsx
+++ b/InputData/endo-learn/BGBSC/BAU Global Battery Storage Cap.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganMahajan\Documents\eps-us\InputData\endo-learn\BGBSC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Modeling\EPS\EU\eps-eu\InputData\endo-learn\BGBSC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CF225A-7568-4778-89A3-1CD84988F734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E264E2-BE6A-4E41-BB81-4FD799660781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="58575" yWindow="1170" windowWidth="27375" windowHeight="15225" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -2839,21 +2839,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="60.85546875" customWidth="1"/>
+    <col min="2" max="2" width="60.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -2861,62 +2861,62 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B5" s="9">
         <v>2024</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B8" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B12" s="9">
         <v>2024</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B13" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B14" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
     </row>
   </sheetData>
@@ -2933,12 +2933,12 @@
       <selection activeCell="B5" sqref="B5:AF5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.140625" customWidth="1"/>
+    <col min="1" max="1" width="35.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="17" t="s">
         <v>21</v>
       </c>
@@ -2946,10 +2946,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" s="17"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>2020</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -3142,7 +3142,7 @@
         <v>3018.3651290394619</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -3284,26 +3284,26 @@
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="48.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" customWidth="1"/>
-    <col min="3" max="3" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="15" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="25" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="29" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.7265625" customWidth="1"/>
+    <col min="3" max="3" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="9" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="10" max="15" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7265625" bestFit="1" customWidth="1"/>
+    <col min="20" max="25" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="27" max="29" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="30" max="31" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="5"/>
       <c r="C1" s="5"/>
@@ -3311,7 +3311,7 @@
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>2020</v>
       </c>
@@ -3334,7 +3334,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>18</v>
       </c>
@@ -3360,12 +3360,12 @@
         <v>3630152910.6631694</v>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>19</v>
       </c>
@@ -3463,7 +3463,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>3630.1529106631624</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -3617,7 +3617,7 @@
       <c r="U13" s="7"/>
       <c r="V13" s="7"/>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -3746,7 +3746,7 @@
         <v>81549620.895449489</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B15" s="12"/>
       <c r="C15" s="12"/>
       <c r="D15" s="14">
@@ -3790,7 +3790,7 @@
       <c r="AE15" s="12"/>
       <c r="AF15" s="12"/>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B16" s="8">
         <f t="shared" ref="B16:AF16" si="1" xml:space="preserve"> (83.94318 + (-3.575905 - 83.94318)/(1 + (B11/2030.462)^372.9304))*1000000</f>
         <v>7551143.5426923158</v>
@@ -3928,34 +3928,34 @@
   <dimension ref="A1:AG15"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="67.42578125" customWidth="1"/>
-    <col min="2" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.453125" customWidth="1"/>
+    <col min="2" max="3" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="7" max="32" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>2020</v>
       </c>
@@ -4050,7 +4050,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -4179,17 +4179,17 @@
         <v>12073460.516157847</v>
       </c>
     </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>2020</v>
       </c>
@@ -4284,7 +4284,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -4414,7 +4414,7 @@
       </c>
       <c r="AG12" s="16"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -4543,7 +4543,7 @@
         <v>84210167.376524493</v>
       </c>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.35">
       <c r="AF15" s="16"/>
     </row>
   </sheetData>
@@ -4564,25 +4564,25 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7265625" customWidth="1"/>
+    <col min="2" max="2" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="8">
-        <f>Summary!B6+Summary!B13</f>
-        <v>203071.80332911675</v>
+        <f>Summary!C6+Summary!C13</f>
+        <v>563553.04625794571</v>
       </c>
     </row>
   </sheetData>
@@ -4595,232 +4595,225 @@
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:AE2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="33" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.7265625" customWidth="1"/>
+    <col min="2" max="10" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="32" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.35">
       <c r="B1">
-        <v>2021</v>
+        <v>2022</v>
       </c>
       <c r="C1">
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="D1">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="E1">
-        <v>2024</v>
+        <v>2025</v>
       </c>
       <c r="F1">
-        <v>2025</v>
+        <v>2026</v>
       </c>
       <c r="G1">
-        <v>2026</v>
+        <v>2027</v>
       </c>
       <c r="H1">
-        <v>2027</v>
+        <v>2028</v>
       </c>
       <c r="I1">
-        <v>2028</v>
+        <v>2029</v>
       </c>
       <c r="J1">
-        <v>2029</v>
+        <v>2030</v>
       </c>
       <c r="K1">
-        <v>2030</v>
+        <v>2031</v>
       </c>
       <c r="L1">
-        <v>2031</v>
+        <v>2032</v>
       </c>
       <c r="M1">
-        <v>2032</v>
+        <v>2033</v>
       </c>
       <c r="N1">
-        <v>2033</v>
+        <v>2034</v>
       </c>
       <c r="O1">
-        <v>2034</v>
+        <v>2035</v>
       </c>
       <c r="P1">
-        <v>2035</v>
+        <v>2036</v>
       </c>
       <c r="Q1">
-        <v>2036</v>
+        <v>2037</v>
       </c>
       <c r="R1">
-        <v>2037</v>
+        <v>2038</v>
       </c>
       <c r="S1">
-        <v>2038</v>
+        <v>2039</v>
       </c>
       <c r="T1">
-        <v>2039</v>
+        <v>2040</v>
       </c>
       <c r="U1">
-        <v>2040</v>
+        <v>2041</v>
       </c>
       <c r="V1">
-        <v>2041</v>
+        <v>2042</v>
       </c>
       <c r="W1">
-        <v>2042</v>
+        <v>2043</v>
       </c>
       <c r="X1">
-        <v>2043</v>
+        <v>2044</v>
       </c>
       <c r="Y1">
-        <v>2044</v>
+        <v>2045</v>
       </c>
       <c r="Z1">
-        <v>2045</v>
+        <v>2046</v>
       </c>
       <c r="AA1">
-        <v>2046</v>
+        <v>2047</v>
       </c>
       <c r="AB1">
-        <v>2047</v>
+        <v>2048</v>
       </c>
       <c r="AC1">
-        <v>2048</v>
+        <v>2049</v>
       </c>
       <c r="AD1">
-        <v>2049</v>
-      </c>
-      <c r="AE1">
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="8">
-        <f>Summary!C6+Summary!C13</f>
-        <v>563553.04625794571</v>
-      </c>
-      <c r="C2" s="8">
         <f>Summary!D6+Summary!D13</f>
         <v>1128822.2416659819</v>
       </c>
-      <c r="D2" s="8">
+      <c r="C2" s="8">
         <f>Summary!E6+Summary!E13</f>
         <v>1952167.6732656616</v>
       </c>
-      <c r="E2" s="8">
+      <c r="D2" s="8">
         <f>Summary!F6+Summary!F13</f>
         <v>2989340.257733738</v>
       </c>
-      <c r="F2" s="8">
+      <c r="E2" s="8">
         <f>Summary!G6+Summary!G13</f>
         <v>4302778.479503056</v>
       </c>
-      <c r="G2" s="8">
+      <c r="F2" s="8">
         <f>Summary!H6+Summary!H13</f>
         <v>5895087.767084918</v>
       </c>
-      <c r="H2" s="8">
+      <c r="G2" s="8">
         <f>Summary!I6+Summary!I13</f>
         <v>7765175.9344945</v>
       </c>
-      <c r="I2" s="8">
+      <c r="H2" s="8">
         <f>Summary!J6+Summary!J13</f>
         <v>9933361.4373499118</v>
       </c>
-      <c r="J2" s="8">
+      <c r="I2" s="8">
         <f>Summary!K6+Summary!K13</f>
         <v>12405442.404781237</v>
       </c>
-      <c r="K2" s="8">
+      <c r="J2" s="8">
         <f>Summary!L6+Summary!L13</f>
         <v>15121253.751472879</v>
       </c>
-      <c r="L2" s="8">
+      <c r="K2" s="8">
         <f>Summary!M6+Summary!M13</f>
         <v>18090409.494550932</v>
       </c>
-      <c r="M2" s="8">
+      <c r="L2" s="8">
         <f>Summary!N6+Summary!N13</f>
         <v>21360659.656938754</v>
       </c>
-      <c r="N2" s="8">
+      <c r="M2" s="8">
         <f>Summary!O6+Summary!O13</f>
         <v>24947950.986543741</v>
       </c>
-      <c r="O2" s="8">
+      <c r="N2" s="8">
         <f>Summary!P6+Summary!P13</f>
         <v>28686641.721218903</v>
       </c>
-      <c r="P2" s="8">
+      <c r="O2" s="8">
         <f>Summary!Q6+Summary!Q13</f>
         <v>32731982.49486623</v>
       </c>
-      <c r="Q2" s="8">
+      <c r="P2" s="8">
         <f>Summary!R6+Summary!R13</f>
         <v>36861203.416973077</v>
       </c>
-      <c r="R2" s="8">
+      <c r="Q2" s="8">
         <f>Summary!S6+Summary!S13</f>
         <v>41049793.134392671</v>
       </c>
-      <c r="S2" s="8">
+      <c r="R2" s="8">
         <f>Summary!T6+Summary!T13</f>
         <v>45381976.654247381</v>
       </c>
-      <c r="T2" s="8">
+      <c r="S2" s="8">
         <f>Summary!U6+Summary!U13</f>
         <v>49796953.051588126</v>
       </c>
-      <c r="U2" s="8">
+      <c r="T2" s="8">
         <f>Summary!V6+Summary!V13</f>
         <v>54207775.935329787</v>
       </c>
-      <c r="V2" s="8">
+      <c r="U2" s="8">
         <f>Summary!W6+Summary!W13</f>
         <v>58478141.490302265</v>
       </c>
-      <c r="W2" s="8">
+      <c r="V2" s="8">
         <f>Summary!X6+Summary!X13</f>
         <v>62765070.801009819</v>
       </c>
-      <c r="X2" s="8">
+      <c r="W2" s="8">
         <f>Summary!Y6+Summary!Y13</f>
         <v>67059206.211048052</v>
       </c>
-      <c r="Y2" s="8">
+      <c r="X2" s="8">
         <f>Summary!Z6+Summary!Z13</f>
         <v>71337882.192170486</v>
       </c>
-      <c r="Z2" s="8">
+      <c r="Y2" s="8">
         <f>Summary!AA6+Summary!AA13</f>
         <v>75666065.641893238</v>
       </c>
-      <c r="AA2" s="8">
+      <c r="Z2" s="8">
         <f>Summary!AB6+Summary!AB13</f>
         <v>79831791.78167291</v>
       </c>
-      <c r="AB2" s="8">
+      <c r="AA2" s="8">
         <f>Summary!AC6+Summary!AC13</f>
         <v>84010308.529606074</v>
       </c>
-      <c r="AC2" s="8">
+      <c r="AB2" s="8">
         <f>Summary!AD6+Summary!AD13</f>
         <v>88133417.808903471</v>
       </c>
-      <c r="AD2" s="8">
+      <c r="AC2" s="8">
         <f>Summary!AE6+Summary!AE13</f>
         <v>92243314.819896087</v>
       </c>
-      <c r="AE2" s="8">
+      <c r="AD2" s="8">
         <f>Summary!AF6+Summary!AF13</f>
         <v>96283627.892682344</v>
       </c>

</xml_diff>